<commit_message>
Revert H2 production shares back to BAU
</commit_message>
<xml_diff>
--- a/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
+++ b/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\hydgn\BHPSbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\hydgn\BHPSbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF5E899-2AC2-40FF-8FAB-92AFAAF5C546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D156AC-81FE-47F0-B74E-85FDE3EE087B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23430" yWindow="3990" windowWidth="23505" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -371,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -381,80 +381,79 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -855,16 +854,15 @@
   </sheetPr>
   <dimension ref="A1:AL938"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:AG51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="114.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -992,7 +990,7 @@
       <c r="AL3" s="7"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6"/>
@@ -1035,7 +1033,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="7"/>
@@ -1077,9 +1075,9 @@
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <f>O51</f>
-        <v>0.75560000000000005</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1117,7 +1115,7 @@
       <c r="AJ6" s="7"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1157,7 +1155,7 @@
       <c r="AL7" s="7"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="7"/>
@@ -1281,7 +1279,7 @@
       <c r="AL10" s="7"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="6"/>
@@ -1323,73 +1321,73 @@
       <c r="AL11" s="7"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
-      <c r="AG12" s="14"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="14"/>
-      <c r="AJ12" s="14"/>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="13"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15" t="s">
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="28" t="s">
         <v>36</v>
       </c>
       <c r="L13" s="7"/>
@@ -1421,27 +1419,27 @@
       <c r="AL13" s="7"/>
     </row>
     <row r="14" spans="1:38" ht="150" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="17" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -1480,32 +1478,32 @@
       <c r="C15" s="7">
         <v>4.7230394679999996</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="15">
         <v>636000000000000</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="15">
         <v>206000000000000</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="15">
         <v>488000000000000</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>3.5</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="17">
         <v>472000000000000</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="17">
         <v>165000000000000</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="15">
         <v>206000000000000</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="15">
         <v>488000000000000</v>
       </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="12">
+      <c r="M15" s="11">
         <v>61493</v>
       </c>
       <c r="N15" s="7" t="s">
@@ -1546,32 +1544,32 @@
       <c r="C16" s="7">
         <v>2.7</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>292000000000000</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="16">
         <v>0</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="15">
         <v>292000000000000</v>
       </c>
       <c r="G16" s="7">
         <v>1.65</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="15">
         <v>222000000000000</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="15">
         <v>69600000000000</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="15">
         <v>222000000000000</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="15">
         <v>69600000000000</v>
       </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="12">
+      <c r="M16" s="11">
         <v>135568.85889999999</v>
       </c>
       <c r="N16" s="7" t="s">
@@ -1612,32 +1610,32 @@
       <c r="C17" s="7">
         <v>1.6</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>173000000000000</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="15">
         <v>173000000000000</v>
       </c>
       <c r="G17" s="7">
         <v>0.27</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <v>36400000000000</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <v>137000000000000</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="15">
         <v>36400000000000</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="15">
         <v>137000000000000</v>
       </c>
       <c r="L17" s="7"/>
-      <c r="M17" s="21">
+      <c r="M17" s="18">
         <v>4110000000</v>
       </c>
       <c r="N17" s="7" t="s">
@@ -1678,38 +1676,38 @@
       <c r="C18" s="7">
         <v>0.2</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="15">
         <v>20800000000000</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="16">
         <v>0</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="15">
         <v>20800000000000</v>
       </c>
       <c r="G18" s="7">
         <v>9.3333333000000004E-2</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="15">
         <v>12600000000000</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="15">
         <v>8210000000000</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="15">
         <v>12600000000000</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="15">
         <v>8210000000000</v>
       </c>
       <c r="L18" s="7"/>
-      <c r="M18" s="12">
+      <c r="M18" s="11">
         <v>50</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="11">
         <v>0.79465919630000004</v>
       </c>
       <c r="P18" s="7"/>
@@ -1746,32 +1744,32 @@
       <c r="C19" s="7">
         <v>0.4</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="15">
         <v>43300000000000</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="16">
         <v>0</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="15">
         <v>43300000000000</v>
       </c>
       <c r="G19" s="7">
         <v>0.18666666700000001</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="15">
         <v>25200000000000</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="15">
         <v>18100000000000</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="15">
         <v>25200000000000</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="15">
         <v>18100000000000</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="M19" s="21">
+      <c r="M19" s="18">
         <v>206000000</v>
       </c>
       <c r="N19" s="7" t="s">
@@ -1843,55 +1841,55 @@
       <c r="AL20" s="7"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
-      <c r="AC21" s="14"/>
-      <c r="AD21" s="14"/>
-      <c r="AE21" s="14"/>
-      <c r="AF21" s="14"/>
-      <c r="AG21" s="14"/>
-      <c r="AH21" s="14"/>
-      <c r="AI21" s="14"/>
-      <c r="AJ21" s="14"/>
-      <c r="AK21" s="14"/>
-      <c r="AL21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="13"/>
+      <c r="AL21" s="13"/>
     </row>
     <row r="22" spans="1:38" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="11">
         <v>75161</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="7"/>
@@ -1931,13 +1929,13 @@
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:38" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="A23" s="11">
         <v>6.2869999999999999</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="21" t="s">
         <v>58</v>
       </c>
       <c r="D23" s="7"/>
@@ -1977,10 +1975,10 @@
       <c r="AL23" s="7"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24" s="18">
         <v>473000000000000</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="22" t="s">
         <v>59</v>
       </c>
       <c r="C24" s="7"/>
@@ -2021,13 +2019,13 @@
       <c r="AL24" s="7"/>
     </row>
     <row r="25" spans="1:38" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+      <c r="A25" s="11">
         <v>199050</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="21" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="7"/>
@@ -2067,7 +2065,7 @@
       <c r="AL25" s="7"/>
     </row>
     <row r="26" spans="1:38" ht="39" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>1037000000</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2111,10 +2109,10 @@
       <c r="AL26" s="7"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="21">
+      <c r="A27" s="18">
         <v>206000000000000</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="7"/>
@@ -2155,13 +2153,13 @@
       <c r="AL27" s="7"/>
     </row>
     <row r="28" spans="1:38" ht="39" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="19">
         <v>0.72</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="21" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="7"/>
@@ -2201,7 +2199,7 @@
       <c r="AL28" s="7"/>
     </row>
     <row r="29" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
+      <c r="A29" s="18">
         <v>149000000000000</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -2245,7 +2243,7 @@
       <c r="AL29" s="7"/>
     </row>
     <row r="30" spans="1:38" ht="39" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
+      <c r="A30" s="20">
         <v>0.23930000000000001</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -2329,142 +2327,142 @@
       <c r="AL31" s="7"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="14"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="14"/>
-      <c r="Z32" s="14"/>
-      <c r="AA32" s="14"/>
-      <c r="AB32" s="14"/>
-      <c r="AC32" s="14"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="14"/>
-      <c r="AF32" s="14"/>
-      <c r="AG32" s="14"/>
-      <c r="AH32" s="14"/>
-      <c r="AI32" s="14"/>
-      <c r="AJ32" s="14"/>
-      <c r="AK32" s="14"/>
-      <c r="AL32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+      <c r="AH32" s="13"/>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="13"/>
+      <c r="AK32" s="13"/>
+      <c r="AL32" s="13"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="24">
         <v>2020</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="24">
         <v>2021</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="24">
         <v>2022</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="24">
         <v>2023</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="24">
         <v>2024</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="24">
         <v>2025</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H33" s="24">
         <v>2026</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="24">
         <v>2027</v>
       </c>
-      <c r="J33" s="27">
+      <c r="J33" s="24">
         <v>2028</v>
       </c>
-      <c r="K33" s="27">
+      <c r="K33" s="24">
         <v>2029</v>
       </c>
-      <c r="L33" s="12">
+      <c r="L33" s="11">
         <v>2030</v>
       </c>
-      <c r="M33" s="12">
+      <c r="M33" s="11">
         <v>2031</v>
       </c>
-      <c r="N33" s="12">
+      <c r="N33" s="11">
         <v>2032</v>
       </c>
-      <c r="O33" s="12">
+      <c r="O33" s="11">
         <v>2033</v>
       </c>
-      <c r="P33" s="12">
+      <c r="P33" s="11">
         <v>2034</v>
       </c>
-      <c r="Q33" s="12">
+      <c r="Q33" s="11">
         <v>2035</v>
       </c>
-      <c r="R33" s="12">
+      <c r="R33" s="11">
         <v>2036</v>
       </c>
-      <c r="S33" s="12">
+      <c r="S33" s="11">
         <v>2037</v>
       </c>
-      <c r="T33" s="12">
+      <c r="T33" s="11">
         <v>2038</v>
       </c>
-      <c r="U33" s="12">
+      <c r="U33" s="11">
         <v>2039</v>
       </c>
-      <c r="V33" s="12">
+      <c r="V33" s="11">
         <v>2040</v>
       </c>
-      <c r="W33" s="12">
+      <c r="W33" s="11">
         <v>2041</v>
       </c>
-      <c r="X33" s="12">
+      <c r="X33" s="11">
         <v>2042</v>
       </c>
-      <c r="Y33" s="12">
+      <c r="Y33" s="11">
         <v>2043</v>
       </c>
-      <c r="Z33" s="12">
+      <c r="Z33" s="11">
         <v>2044</v>
       </c>
-      <c r="AA33" s="12">
+      <c r="AA33" s="11">
         <v>2045</v>
       </c>
-      <c r="AB33" s="12">
+      <c r="AB33" s="11">
         <v>2046</v>
       </c>
-      <c r="AC33" s="12">
+      <c r="AC33" s="11">
         <v>2047</v>
       </c>
-      <c r="AD33" s="12">
+      <c r="AD33" s="11">
         <v>2048</v>
       </c>
-      <c r="AE33" s="12">
+      <c r="AE33" s="11">
         <v>2049</v>
       </c>
-      <c r="AF33" s="12">
+      <c r="AF33" s="11">
         <v>2050</v>
       </c>
       <c r="AG33" s="7"/>
@@ -2475,100 +2473,100 @@
       <c r="AL33" s="7"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="15">
         <v>488000000000000</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="15">
         <v>553000000000000</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="15">
         <v>572000000000000</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="15">
         <v>582000000000000</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="15">
         <v>588000000000000</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="15">
         <v>590000000000000</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="15">
         <v>591000000000000</v>
       </c>
-      <c r="I34" s="18">
+      <c r="I34" s="15">
         <v>590000000000000</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="15">
         <v>588000000000000</v>
       </c>
-      <c r="K34" s="18">
+      <c r="K34" s="15">
         <v>588000000000000</v>
       </c>
-      <c r="L34" s="21">
+      <c r="L34" s="18">
         <v>588000000000000</v>
       </c>
-      <c r="M34" s="21">
+      <c r="M34" s="18">
         <v>583000000000000</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="18">
         <v>583000000000000</v>
       </c>
-      <c r="O34" s="21">
+      <c r="O34" s="18">
         <v>581000000000000</v>
       </c>
-      <c r="P34" s="21">
+      <c r="P34" s="18">
         <v>581000000000000</v>
       </c>
-      <c r="Q34" s="21">
+      <c r="Q34" s="18">
         <v>580000000000000</v>
       </c>
-      <c r="R34" s="21">
+      <c r="R34" s="18">
         <v>580000000000000</v>
       </c>
-      <c r="S34" s="21">
+      <c r="S34" s="18">
         <v>581000000000000</v>
       </c>
-      <c r="T34" s="21">
+      <c r="T34" s="18">
         <v>581000000000000</v>
       </c>
-      <c r="U34" s="21">
+      <c r="U34" s="18">
         <v>582000000000000</v>
       </c>
-      <c r="V34" s="21">
+      <c r="V34" s="18">
         <v>580000000000000</v>
       </c>
-      <c r="W34" s="21">
+      <c r="W34" s="18">
         <v>581000000000000</v>
       </c>
-      <c r="X34" s="21">
+      <c r="X34" s="18">
         <v>580000000000000</v>
       </c>
-      <c r="Y34" s="21">
+      <c r="Y34" s="18">
         <v>578000000000000</v>
       </c>
-      <c r="Z34" s="21">
+      <c r="Z34" s="18">
         <v>578000000000000</v>
       </c>
-      <c r="AA34" s="21">
+      <c r="AA34" s="18">
         <v>577000000000000</v>
       </c>
-      <c r="AB34" s="21">
+      <c r="AB34" s="18">
         <v>575000000000000</v>
       </c>
-      <c r="AC34" s="21">
+      <c r="AC34" s="18">
         <v>576000000000000</v>
       </c>
-      <c r="AD34" s="21">
+      <c r="AD34" s="18">
         <v>573000000000000</v>
       </c>
-      <c r="AE34" s="21">
+      <c r="AE34" s="18">
         <v>572000000000000</v>
       </c>
-      <c r="AF34" s="21">
+      <c r="AF34" s="18">
         <v>574000000000000</v>
       </c>
       <c r="AG34" s="7"/>
@@ -2579,100 +2577,100 @@
       <c r="AL34" s="7"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="15">
         <v>224000000000000</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="15">
         <v>227000000000000</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="15">
         <v>252000000000000</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="15">
         <v>270000000000000</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="15">
         <v>278000000000000</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="15">
         <v>284000000000000</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H35" s="15">
         <v>288000000000000</v>
       </c>
-      <c r="I35" s="18">
+      <c r="I35" s="15">
         <v>290000000000000</v>
       </c>
-      <c r="J35" s="18">
+      <c r="J35" s="15">
         <v>294000000000000</v>
       </c>
-      <c r="K35" s="18">
+      <c r="K35" s="15">
         <v>297000000000000</v>
       </c>
-      <c r="L35" s="21">
+      <c r="L35" s="18">
         <v>301000000000000</v>
       </c>
-      <c r="M35" s="21">
+      <c r="M35" s="18">
         <v>305000000000000</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="18">
         <v>308000000000000</v>
       </c>
-      <c r="O35" s="21">
+      <c r="O35" s="18">
         <v>311000000000000</v>
       </c>
-      <c r="P35" s="21">
+      <c r="P35" s="18">
         <v>315000000000000</v>
       </c>
-      <c r="Q35" s="21">
+      <c r="Q35" s="18">
         <v>319000000000000</v>
       </c>
-      <c r="R35" s="21">
+      <c r="R35" s="18">
         <v>323000000000000</v>
       </c>
-      <c r="S35" s="21">
+      <c r="S35" s="18">
         <v>326000000000000</v>
       </c>
-      <c r="T35" s="21">
+      <c r="T35" s="18">
         <v>329000000000000</v>
       </c>
-      <c r="U35" s="21">
+      <c r="U35" s="18">
         <v>332000000000000</v>
       </c>
-      <c r="V35" s="21">
+      <c r="V35" s="18">
         <v>333000000000000</v>
       </c>
-      <c r="W35" s="21">
+      <c r="W35" s="18">
         <v>334000000000000</v>
       </c>
-      <c r="X35" s="21">
+      <c r="X35" s="18">
         <v>336000000000000</v>
       </c>
-      <c r="Y35" s="21">
+      <c r="Y35" s="18">
         <v>340000000000000</v>
       </c>
-      <c r="Z35" s="21">
+      <c r="Z35" s="18">
         <v>343000000000000</v>
       </c>
-      <c r="AA35" s="21">
+      <c r="AA35" s="18">
         <v>347000000000000</v>
       </c>
-      <c r="AB35" s="21">
+      <c r="AB35" s="18">
         <v>349000000000000</v>
       </c>
-      <c r="AC35" s="21">
+      <c r="AC35" s="18">
         <v>351000000000000</v>
       </c>
-      <c r="AD35" s="21">
+      <c r="AD35" s="18">
         <v>352000000000000</v>
       </c>
-      <c r="AE35" s="21">
+      <c r="AE35" s="18">
         <v>355000000000000</v>
       </c>
-      <c r="AF35" s="21">
+      <c r="AF35" s="18">
         <v>359000000000000</v>
       </c>
       <c r="AG35" s="7"/>
@@ -2683,100 +2681,100 @@
       <c r="AL35" s="7"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="15">
         <v>8210000000000</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="15">
         <v>7150000000000</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="15">
         <v>7970000000000</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="15">
         <v>7740000000000</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="15">
         <v>7940000000000</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="15">
         <v>8320000000000</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="15">
         <v>8170000000000</v>
       </c>
-      <c r="I36" s="18">
+      <c r="I36" s="15">
         <v>8030000000000</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="15">
         <v>7900000000000</v>
       </c>
-      <c r="K36" s="18">
+      <c r="K36" s="15">
         <v>7820000000000</v>
       </c>
-      <c r="L36" s="21">
+      <c r="L36" s="18">
         <v>7780000000000</v>
       </c>
-      <c r="M36" s="21">
+      <c r="M36" s="18">
         <v>7300000000000</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="18">
         <v>6840000000000</v>
       </c>
-      <c r="O36" s="21">
+      <c r="O36" s="18">
         <v>6400000000000</v>
       </c>
-      <c r="P36" s="21">
+      <c r="P36" s="18">
         <v>6120000000000</v>
       </c>
-      <c r="Q36" s="21">
+      <c r="Q36" s="18">
         <v>6040000000000</v>
       </c>
-      <c r="R36" s="21">
+      <c r="R36" s="18">
         <v>5980000000000</v>
       </c>
-      <c r="S36" s="21">
+      <c r="S36" s="18">
         <v>5960000000000</v>
       </c>
-      <c r="T36" s="21">
+      <c r="T36" s="18">
         <v>6000000000000</v>
       </c>
-      <c r="U36" s="21">
+      <c r="U36" s="18">
         <v>6050000000000</v>
       </c>
-      <c r="V36" s="21">
+      <c r="V36" s="18">
         <v>6000000000000</v>
       </c>
-      <c r="W36" s="21">
+      <c r="W36" s="18">
         <v>6000000000000</v>
       </c>
-      <c r="X36" s="21">
+      <c r="X36" s="18">
         <v>6090000000000</v>
       </c>
-      <c r="Y36" s="21">
+      <c r="Y36" s="18">
         <v>6260000000000</v>
       </c>
-      <c r="Z36" s="21">
+      <c r="Z36" s="18">
         <v>6270000000000</v>
       </c>
-      <c r="AA36" s="21">
+      <c r="AA36" s="18">
         <v>6340000000000</v>
       </c>
-      <c r="AB36" s="21">
+      <c r="AB36" s="18">
         <v>6340000000000</v>
       </c>
-      <c r="AC36" s="21">
+      <c r="AC36" s="18">
         <v>6300000000000</v>
       </c>
-      <c r="AD36" s="21">
+      <c r="AD36" s="18">
         <v>6340000000000</v>
       </c>
-      <c r="AE36" s="21">
+      <c r="AE36" s="18">
         <v>6390000000000</v>
       </c>
-      <c r="AF36" s="21">
+      <c r="AF36" s="18">
         <v>6540000000000</v>
       </c>
       <c r="AG36" s="7"/>
@@ -2787,17 +2785,17 @@
       <c r="AL36" s="7"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
@@ -2827,145 +2825,145 @@
       <c r="AL37" s="7"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
-      <c r="W38" s="14"/>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="14"/>
-      <c r="Z38" s="14"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AC38" s="14"/>
-      <c r="AD38" s="14"/>
-      <c r="AE38" s="14"/>
-      <c r="AF38" s="14"/>
-      <c r="AG38" s="14"/>
-      <c r="AH38" s="14"/>
-      <c r="AI38" s="14"/>
-      <c r="AJ38" s="14"/>
-      <c r="AK38" s="14"/>
-      <c r="AL38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="13"/>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="13"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="25">
         <v>2020</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="25">
         <v>2021</v>
       </c>
-      <c r="E39" s="28">
+      <c r="E39" s="25">
         <v>2022</v>
       </c>
-      <c r="F39" s="28">
+      <c r="F39" s="25">
         <v>2023</v>
       </c>
-      <c r="G39" s="28">
+      <c r="G39" s="25">
         <v>2024</v>
       </c>
-      <c r="H39" s="28">
+      <c r="H39" s="25">
         <v>2025</v>
       </c>
-      <c r="I39" s="28">
+      <c r="I39" s="25">
         <v>2026</v>
       </c>
-      <c r="J39" s="28">
+      <c r="J39" s="25">
         <v>2027</v>
       </c>
-      <c r="K39" s="28">
+      <c r="K39" s="25">
         <v>2028</v>
       </c>
-      <c r="L39" s="28">
+      <c r="L39" s="25">
         <v>2029</v>
       </c>
-      <c r="M39" s="28">
+      <c r="M39" s="25">
         <v>2030</v>
       </c>
-      <c r="N39" s="28">
+      <c r="N39" s="25">
         <v>2031</v>
       </c>
-      <c r="O39" s="28">
+      <c r="O39" s="25">
         <v>2032</v>
       </c>
-      <c r="P39" s="28">
+      <c r="P39" s="25">
         <v>2033</v>
       </c>
-      <c r="Q39" s="28">
+      <c r="Q39" s="25">
         <v>2034</v>
       </c>
-      <c r="R39" s="28">
+      <c r="R39" s="25">
         <v>2035</v>
       </c>
-      <c r="S39" s="28">
+      <c r="S39" s="25">
         <v>2036</v>
       </c>
-      <c r="T39" s="28">
+      <c r="T39" s="25">
         <v>2037</v>
       </c>
-      <c r="U39" s="28">
+      <c r="U39" s="25">
         <v>2038</v>
       </c>
-      <c r="V39" s="28">
+      <c r="V39" s="25">
         <v>2039</v>
       </c>
-      <c r="W39" s="28">
+      <c r="W39" s="25">
         <v>2040</v>
       </c>
-      <c r="X39" s="28">
+      <c r="X39" s="25">
         <v>2041</v>
       </c>
-      <c r="Y39" s="28">
+      <c r="Y39" s="25">
         <v>2042</v>
       </c>
-      <c r="Z39" s="28">
+      <c r="Z39" s="25">
         <v>2043</v>
       </c>
-      <c r="AA39" s="28">
+      <c r="AA39" s="25">
         <v>2044</v>
       </c>
-      <c r="AB39" s="28">
+      <c r="AB39" s="25">
         <v>2045</v>
       </c>
-      <c r="AC39" s="28">
+      <c r="AC39" s="25">
         <v>2046</v>
       </c>
-      <c r="AD39" s="28">
+      <c r="AD39" s="25">
         <v>2047</v>
       </c>
-      <c r="AE39" s="28">
+      <c r="AE39" s="25">
         <v>2048</v>
       </c>
-      <c r="AF39" s="28">
+      <c r="AF39" s="25">
         <v>2049</v>
       </c>
-      <c r="AG39" s="28">
+      <c r="AG39" s="25">
         <v>2050</v>
       </c>
       <c r="AH39" s="7"/>
@@ -2981,97 +2979,97 @@
       <c r="B40" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="11">
         <v>0</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="11">
         <v>0</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="19">
         <v>0.11</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="19">
         <v>0.22</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="19">
         <v>0.33</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="19">
         <v>0.44</v>
       </c>
-      <c r="I40" s="22">
+      <c r="I40" s="19">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J40" s="22">
+      <c r="J40" s="19">
         <v>0.67</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="19">
         <v>0.78</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="19">
         <v>0.89</v>
       </c>
-      <c r="M40" s="22">
+      <c r="M40" s="19">
         <v>1</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N40" s="19">
         <v>1</v>
       </c>
-      <c r="O40" s="22">
+      <c r="O40" s="19">
         <v>1</v>
       </c>
-      <c r="P40" s="22">
+      <c r="P40" s="19">
         <v>1</v>
       </c>
-      <c r="Q40" s="22">
+      <c r="Q40" s="19">
         <v>1</v>
       </c>
-      <c r="R40" s="22">
+      <c r="R40" s="19">
         <v>1</v>
       </c>
-      <c r="S40" s="22">
+      <c r="S40" s="19">
         <v>1</v>
       </c>
-      <c r="T40" s="22">
+      <c r="T40" s="19">
         <v>1</v>
       </c>
-      <c r="U40" s="22">
+      <c r="U40" s="19">
         <v>1</v>
       </c>
-      <c r="V40" s="22">
+      <c r="V40" s="19">
         <v>1</v>
       </c>
-      <c r="W40" s="22">
+      <c r="W40" s="19">
         <v>1</v>
       </c>
-      <c r="X40" s="22">
+      <c r="X40" s="19">
         <v>1</v>
       </c>
-      <c r="Y40" s="22">
+      <c r="Y40" s="19">
         <v>1</v>
       </c>
-      <c r="Z40" s="22">
+      <c r="Z40" s="19">
         <v>1</v>
       </c>
-      <c r="AA40" s="22">
+      <c r="AA40" s="19">
         <v>1</v>
       </c>
-      <c r="AB40" s="22">
+      <c r="AB40" s="19">
         <v>1</v>
       </c>
-      <c r="AC40" s="22">
+      <c r="AC40" s="19">
         <v>1</v>
       </c>
-      <c r="AD40" s="22">
+      <c r="AD40" s="19">
         <v>1</v>
       </c>
-      <c r="AE40" s="22">
+      <c r="AE40" s="19">
         <v>1</v>
       </c>
-      <c r="AF40" s="22">
+      <c r="AF40" s="19">
         <v>1</v>
       </c>
-      <c r="AG40" s="22">
+      <c r="AG40" s="19">
         <v>1</v>
       </c>
       <c r="AH40" s="7"/>
@@ -3087,97 +3085,97 @@
       <c r="B41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="11">
         <v>0</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="11">
         <v>0</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="19">
         <v>0.11</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F41" s="19">
         <v>0.22</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="19">
         <v>0.33</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="19">
         <v>0.44</v>
       </c>
-      <c r="I41" s="22">
+      <c r="I41" s="19">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J41" s="22">
+      <c r="J41" s="19">
         <v>0.67</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="19">
         <v>0.78</v>
       </c>
-      <c r="L41" s="22">
+      <c r="L41" s="19">
         <v>0.89</v>
       </c>
-      <c r="M41" s="29">
+      <c r="M41" s="26">
         <v>1</v>
       </c>
-      <c r="N41" s="22">
+      <c r="N41" s="19">
         <v>1</v>
       </c>
-      <c r="O41" s="22">
+      <c r="O41" s="19">
         <v>1</v>
       </c>
-      <c r="P41" s="22">
+      <c r="P41" s="19">
         <v>1</v>
       </c>
-      <c r="Q41" s="22">
+      <c r="Q41" s="19">
         <v>1</v>
       </c>
-      <c r="R41" s="22">
+      <c r="R41" s="19">
         <v>1</v>
       </c>
-      <c r="S41" s="22">
+      <c r="S41" s="19">
         <v>1</v>
       </c>
-      <c r="T41" s="22">
+      <c r="T41" s="19">
         <v>1</v>
       </c>
-      <c r="U41" s="22">
+      <c r="U41" s="19">
         <v>1</v>
       </c>
-      <c r="V41" s="22">
+      <c r="V41" s="19">
         <v>1</v>
       </c>
-      <c r="W41" s="22">
+      <c r="W41" s="19">
         <v>1</v>
       </c>
-      <c r="X41" s="22">
+      <c r="X41" s="19">
         <v>1</v>
       </c>
-      <c r="Y41" s="22">
+      <c r="Y41" s="19">
         <v>1</v>
       </c>
-      <c r="Z41" s="22">
+      <c r="Z41" s="19">
         <v>1</v>
       </c>
-      <c r="AA41" s="22">
+      <c r="AA41" s="19">
         <v>1</v>
       </c>
-      <c r="AB41" s="22">
+      <c r="AB41" s="19">
         <v>1</v>
       </c>
-      <c r="AC41" s="22">
+      <c r="AC41" s="19">
         <v>1</v>
       </c>
-      <c r="AD41" s="22">
+      <c r="AD41" s="19">
         <v>1</v>
       </c>
-      <c r="AE41" s="22">
+      <c r="AE41" s="19">
         <v>1</v>
       </c>
-      <c r="AF41" s="22">
+      <c r="AF41" s="19">
         <v>1</v>
       </c>
-      <c r="AG41" s="22">
+      <c r="AG41" s="19">
         <v>1</v>
       </c>
       <c r="AH41" s="7"/>
@@ -3193,97 +3191,97 @@
       <c r="B42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="11">
         <v>0</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="11">
         <v>0</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="19">
         <v>0</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F42" s="19">
         <v>0</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="19">
         <v>0</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="19">
         <v>0</v>
       </c>
-      <c r="I42" s="22">
+      <c r="I42" s="19">
         <v>0</v>
       </c>
-      <c r="J42" s="22">
+      <c r="J42" s="19">
         <v>0</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K42" s="19">
         <v>0</v>
       </c>
-      <c r="L42" s="22">
+      <c r="L42" s="19">
         <v>0</v>
       </c>
-      <c r="M42" s="12">
+      <c r="M42" s="11">
         <v>0</v>
       </c>
-      <c r="N42" s="12">
+      <c r="N42" s="11">
         <v>0</v>
       </c>
-      <c r="O42" s="12">
+      <c r="O42" s="11">
         <v>0</v>
       </c>
-      <c r="P42" s="12">
+      <c r="P42" s="11">
         <v>0</v>
       </c>
-      <c r="Q42" s="12">
+      <c r="Q42" s="11">
         <v>0</v>
       </c>
-      <c r="R42" s="12">
+      <c r="R42" s="11">
         <v>0</v>
       </c>
-      <c r="S42" s="12">
+      <c r="S42" s="11">
         <v>0</v>
       </c>
-      <c r="T42" s="12">
+      <c r="T42" s="11">
         <v>0</v>
       </c>
-      <c r="U42" s="12">
+      <c r="U42" s="11">
         <v>0</v>
       </c>
-      <c r="V42" s="12">
+      <c r="V42" s="11">
         <v>0</v>
       </c>
-      <c r="W42" s="12">
+      <c r="W42" s="11">
         <v>0</v>
       </c>
-      <c r="X42" s="12">
+      <c r="X42" s="11">
         <v>0</v>
       </c>
-      <c r="Y42" s="12">
+      <c r="Y42" s="11">
         <v>0</v>
       </c>
-      <c r="Z42" s="12">
+      <c r="Z42" s="11">
         <v>0</v>
       </c>
-      <c r="AA42" s="12">
+      <c r="AA42" s="11">
         <v>0</v>
       </c>
-      <c r="AB42" s="12">
+      <c r="AB42" s="11">
         <v>0</v>
       </c>
-      <c r="AC42" s="12">
+      <c r="AC42" s="11">
         <v>0</v>
       </c>
-      <c r="AD42" s="12">
+      <c r="AD42" s="11">
         <v>0</v>
       </c>
-      <c r="AE42" s="12">
+      <c r="AE42" s="11">
         <v>0</v>
       </c>
-      <c r="AF42" s="12">
+      <c r="AF42" s="11">
         <v>0</v>
       </c>
-      <c r="AG42" s="12">
+      <c r="AG42" s="11">
         <v>0</v>
       </c>
       <c r="AH42" s="7"/>
@@ -3299,97 +3297,97 @@
       <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="11">
         <v>0</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="11">
         <v>0</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E43" s="19">
         <v>0</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F43" s="19">
         <v>0</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="19">
         <v>0</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H43" s="19">
         <v>0</v>
       </c>
-      <c r="I43" s="22">
+      <c r="I43" s="19">
         <v>0</v>
       </c>
-      <c r="J43" s="22">
+      <c r="J43" s="19">
         <v>0</v>
       </c>
-      <c r="K43" s="22">
+      <c r="K43" s="19">
         <v>0</v>
       </c>
-      <c r="L43" s="22">
+      <c r="L43" s="19">
         <v>0</v>
       </c>
-      <c r="M43" s="12">
+      <c r="M43" s="11">
         <v>0</v>
       </c>
-      <c r="N43" s="12">
+      <c r="N43" s="11">
         <v>0</v>
       </c>
-      <c r="O43" s="12">
+      <c r="O43" s="11">
         <v>0</v>
       </c>
-      <c r="P43" s="12">
+      <c r="P43" s="11">
         <v>0</v>
       </c>
-      <c r="Q43" s="12">
+      <c r="Q43" s="11">
         <v>0</v>
       </c>
-      <c r="R43" s="12">
+      <c r="R43" s="11">
         <v>0</v>
       </c>
-      <c r="S43" s="12">
+      <c r="S43" s="11">
         <v>0</v>
       </c>
-      <c r="T43" s="12">
+      <c r="T43" s="11">
         <v>0</v>
       </c>
-      <c r="U43" s="12">
+      <c r="U43" s="11">
         <v>0</v>
       </c>
-      <c r="V43" s="12">
+      <c r="V43" s="11">
         <v>0</v>
       </c>
-      <c r="W43" s="12">
+      <c r="W43" s="11">
         <v>0</v>
       </c>
-      <c r="X43" s="12">
+      <c r="X43" s="11">
         <v>0</v>
       </c>
-      <c r="Y43" s="12">
+      <c r="Y43" s="11">
         <v>0</v>
       </c>
-      <c r="Z43" s="12">
+      <c r="Z43" s="11">
         <v>0</v>
       </c>
-      <c r="AA43" s="12">
+      <c r="AA43" s="11">
         <v>0</v>
       </c>
-      <c r="AB43" s="12">
+      <c r="AB43" s="11">
         <v>0</v>
       </c>
-      <c r="AC43" s="12">
+      <c r="AC43" s="11">
         <v>0</v>
       </c>
-      <c r="AD43" s="12">
+      <c r="AD43" s="11">
         <v>0</v>
       </c>
-      <c r="AE43" s="12">
+      <c r="AE43" s="11">
         <v>0</v>
       </c>
-      <c r="AF43" s="12">
+      <c r="AF43" s="11">
         <v>0</v>
       </c>
-      <c r="AG43" s="12">
+      <c r="AG43" s="11">
         <v>0</v>
       </c>
       <c r="AH43" s="7"/>
@@ -3405,97 +3403,97 @@
       <c r="B44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="11">
         <v>0</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="11">
         <v>0</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="19">
         <v>0</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="19">
         <v>0</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="19">
         <v>0</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="19">
         <v>0</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="19">
         <v>0</v>
       </c>
-      <c r="J44" s="22">
+      <c r="J44" s="19">
         <v>0</v>
       </c>
-      <c r="K44" s="22">
+      <c r="K44" s="19">
         <v>0</v>
       </c>
-      <c r="L44" s="22">
+      <c r="L44" s="19">
         <v>0</v>
       </c>
-      <c r="M44" s="12">
+      <c r="M44" s="11">
         <v>0</v>
       </c>
-      <c r="N44" s="12">
+      <c r="N44" s="11">
         <v>0</v>
       </c>
-      <c r="O44" s="12">
+      <c r="O44" s="11">
         <v>0</v>
       </c>
-      <c r="P44" s="12">
+      <c r="P44" s="11">
         <v>0</v>
       </c>
-      <c r="Q44" s="12">
+      <c r="Q44" s="11">
         <v>0</v>
       </c>
-      <c r="R44" s="12">
+      <c r="R44" s="11">
         <v>0</v>
       </c>
-      <c r="S44" s="12">
+      <c r="S44" s="11">
         <v>0</v>
       </c>
-      <c r="T44" s="12">
+      <c r="T44" s="11">
         <v>0</v>
       </c>
-      <c r="U44" s="12">
+      <c r="U44" s="11">
         <v>0</v>
       </c>
-      <c r="V44" s="12">
+      <c r="V44" s="11">
         <v>0</v>
       </c>
-      <c r="W44" s="12">
+      <c r="W44" s="11">
         <v>0</v>
       </c>
-      <c r="X44" s="12">
+      <c r="X44" s="11">
         <v>0</v>
       </c>
-      <c r="Y44" s="12">
+      <c r="Y44" s="11">
         <v>0</v>
       </c>
-      <c r="Z44" s="12">
+      <c r="Z44" s="11">
         <v>0</v>
       </c>
-      <c r="AA44" s="12">
+      <c r="AA44" s="11">
         <v>0</v>
       </c>
-      <c r="AB44" s="12">
+      <c r="AB44" s="11">
         <v>0</v>
       </c>
-      <c r="AC44" s="12">
+      <c r="AC44" s="11">
         <v>0</v>
       </c>
-      <c r="AD44" s="12">
+      <c r="AD44" s="11">
         <v>0</v>
       </c>
-      <c r="AE44" s="12">
+      <c r="AE44" s="11">
         <v>0</v>
       </c>
-      <c r="AF44" s="12">
+      <c r="AF44" s="11">
         <v>0</v>
       </c>
-      <c r="AG44" s="12">
+      <c r="AG44" s="11">
         <v>0</v>
       </c>
       <c r="AH44" s="7"/>
@@ -3545,101 +3543,101 @@
       <c r="AL45" s="7"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="7"/>
-      <c r="C46" s="23">
+      <c r="C46" s="20">
         <v>0</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="20">
         <v>0</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="20">
         <v>0.1111</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <v>0.22220000000000001</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="20">
         <v>0.33329999999999999</v>
       </c>
-      <c r="H46" s="23">
+      <c r="H46" s="20">
         <v>0.44440000000000002</v>
       </c>
-      <c r="I46" s="23">
+      <c r="I46" s="20">
         <v>0.55559999999999998</v>
       </c>
-      <c r="J46" s="23">
+      <c r="J46" s="20">
         <v>0.66669999999999996</v>
       </c>
-      <c r="K46" s="23">
+      <c r="K46" s="20">
         <v>0.77780000000000005</v>
       </c>
-      <c r="L46" s="23">
+      <c r="L46" s="20">
         <v>0.88890000000000002</v>
       </c>
-      <c r="M46" s="23">
+      <c r="M46" s="20">
         <v>1</v>
       </c>
-      <c r="N46" s="23">
+      <c r="N46" s="20">
         <v>1</v>
       </c>
-      <c r="O46" s="23">
+      <c r="O46" s="20">
         <v>1</v>
       </c>
-      <c r="P46" s="23">
+      <c r="P46" s="20">
         <v>1</v>
       </c>
-      <c r="Q46" s="23">
+      <c r="Q46" s="20">
         <v>1</v>
       </c>
-      <c r="R46" s="23">
+      <c r="R46" s="20">
         <v>1</v>
       </c>
-      <c r="S46" s="23">
+      <c r="S46" s="20">
         <v>1</v>
       </c>
-      <c r="T46" s="23">
+      <c r="T46" s="20">
         <v>1</v>
       </c>
-      <c r="U46" s="23">
+      <c r="U46" s="20">
         <v>1</v>
       </c>
-      <c r="V46" s="23">
+      <c r="V46" s="20">
         <v>1</v>
       </c>
-      <c r="W46" s="23">
+      <c r="W46" s="20">
         <v>1</v>
       </c>
-      <c r="X46" s="23">
+      <c r="X46" s="20">
         <v>1</v>
       </c>
-      <c r="Y46" s="23">
+      <c r="Y46" s="20">
         <v>1</v>
       </c>
-      <c r="Z46" s="23">
+      <c r="Z46" s="20">
         <v>1</v>
       </c>
-      <c r="AA46" s="23">
+      <c r="AA46" s="20">
         <v>1</v>
       </c>
-      <c r="AB46" s="23">
+      <c r="AB46" s="20">
         <v>1</v>
       </c>
-      <c r="AC46" s="23">
+      <c r="AC46" s="20">
         <v>1</v>
       </c>
-      <c r="AD46" s="23">
+      <c r="AD46" s="20">
         <v>1</v>
       </c>
-      <c r="AE46" s="23">
+      <c r="AE46" s="20">
         <v>1</v>
       </c>
-      <c r="AF46" s="23">
+      <c r="AF46" s="20">
         <v>1</v>
       </c>
-      <c r="AG46" s="23">
+      <c r="AG46" s="20">
         <v>1</v>
       </c>
       <c r="AH46" s="7"/>
@@ -3649,101 +3647,101 @@
       <c r="AL46" s="7"/>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="7"/>
-      <c r="C47" s="23">
+      <c r="C47" s="20">
         <v>0</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="20">
         <v>0</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="20">
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="20">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="20">
         <v>0.10340000000000001</v>
       </c>
-      <c r="H47" s="23">
+      <c r="H47" s="20">
         <v>0.13789999999999999</v>
       </c>
-      <c r="I47" s="23">
+      <c r="I47" s="20">
         <v>0.1724</v>
       </c>
-      <c r="J47" s="23">
+      <c r="J47" s="20">
         <v>0.20680000000000001</v>
       </c>
-      <c r="K47" s="23">
+      <c r="K47" s="20">
         <v>0.24129999999999999</v>
       </c>
-      <c r="L47" s="23">
+      <c r="L47" s="20">
         <v>0.27579999999999999</v>
       </c>
-      <c r="M47" s="23">
+      <c r="M47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="N47" s="23">
+      <c r="N47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="O47" s="23">
+      <c r="O47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="P47" s="23">
+      <c r="P47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="Q47" s="23">
+      <c r="Q47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="R47" s="23">
+      <c r="R47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="S47" s="23">
+      <c r="S47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="T47" s="23">
+      <c r="T47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="U47" s="23">
+      <c r="U47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="V47" s="23">
+      <c r="V47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="W47" s="23">
+      <c r="W47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="X47" s="23">
+      <c r="X47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="Y47" s="23">
+      <c r="Y47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="Z47" s="23">
+      <c r="Z47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AA47" s="23">
+      <c r="AA47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AB47" s="23">
+      <c r="AB47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AC47" s="23">
+      <c r="AC47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AD47" s="23">
+      <c r="AD47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AE47" s="23">
+      <c r="AE47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AF47" s="23">
+      <c r="AF47" s="20">
         <v>0.31030000000000002</v>
       </c>
-      <c r="AG47" s="23">
+      <c r="AG47" s="20">
         <v>0.31030000000000002</v>
       </c>
       <c r="AH47" s="7"/>
@@ -3753,101 +3751,101 @@
       <c r="AL47" s="7"/>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B48" s="7"/>
-      <c r="C48" s="23">
+      <c r="C48" s="20">
         <v>0</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="20">
         <v>0</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E48" s="20">
         <v>0</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="20">
         <v>0</v>
       </c>
-      <c r="G48" s="23">
+      <c r="G48" s="20">
         <v>0</v>
       </c>
-      <c r="H48" s="23">
+      <c r="H48" s="20">
         <v>0</v>
       </c>
-      <c r="I48" s="23">
+      <c r="I48" s="20">
         <v>0</v>
       </c>
-      <c r="J48" s="23">
+      <c r="J48" s="20">
         <v>0</v>
       </c>
-      <c r="K48" s="23">
+      <c r="K48" s="20">
         <v>0</v>
       </c>
-      <c r="L48" s="23">
+      <c r="L48" s="20">
         <v>0</v>
       </c>
-      <c r="M48" s="23">
+      <c r="M48" s="20">
         <v>0</v>
       </c>
-      <c r="N48" s="23">
+      <c r="N48" s="20">
         <v>0</v>
       </c>
-      <c r="O48" s="23">
+      <c r="O48" s="20">
         <v>0</v>
       </c>
-      <c r="P48" s="23">
+      <c r="P48" s="20">
         <v>0</v>
       </c>
-      <c r="Q48" s="23">
+      <c r="Q48" s="20">
         <v>0</v>
       </c>
-      <c r="R48" s="23">
+      <c r="R48" s="20">
         <v>0</v>
       </c>
-      <c r="S48" s="23">
+      <c r="S48" s="20">
         <v>0</v>
       </c>
-      <c r="T48" s="23">
+      <c r="T48" s="20">
         <v>0</v>
       </c>
-      <c r="U48" s="23">
+      <c r="U48" s="20">
         <v>0</v>
       </c>
-      <c r="V48" s="23">
+      <c r="V48" s="20">
         <v>0</v>
       </c>
-      <c r="W48" s="23">
+      <c r="W48" s="20">
         <v>0</v>
       </c>
-      <c r="X48" s="23">
+      <c r="X48" s="20">
         <v>0</v>
       </c>
-      <c r="Y48" s="23">
+      <c r="Y48" s="20">
         <v>0</v>
       </c>
-      <c r="Z48" s="23">
+      <c r="Z48" s="20">
         <v>0</v>
       </c>
-      <c r="AA48" s="23">
+      <c r="AA48" s="20">
         <v>0</v>
       </c>
-      <c r="AB48" s="23">
+      <c r="AB48" s="20">
         <v>0</v>
       </c>
-      <c r="AC48" s="23">
+      <c r="AC48" s="20">
         <v>0</v>
       </c>
-      <c r="AD48" s="23">
+      <c r="AD48" s="20">
         <v>0</v>
       </c>
-      <c r="AE48" s="23">
+      <c r="AE48" s="20">
         <v>0</v>
       </c>
-      <c r="AF48" s="23">
+      <c r="AF48" s="20">
         <v>0</v>
       </c>
-      <c r="AG48" s="23">
+      <c r="AG48" s="20">
         <v>0</v>
       </c>
       <c r="AH48" s="7"/>
@@ -3941,98 +3939,98 @@
         <v>69</v>
       </c>
       <c r="B51" s="7"/>
-      <c r="C51" s="23">
+      <c r="C51" s="20">
         <v>0</v>
       </c>
-      <c r="D51" s="23">
+      <c r="D51" s="20">
         <v>0</v>
       </c>
-      <c r="E51" s="23">
-        <v>8.6900000000000005E-2</v>
-      </c>
-      <c r="F51" s="23">
-        <v>0.1721</v>
-      </c>
-      <c r="G51" s="23">
-        <v>0.25719999999999998</v>
-      </c>
-      <c r="H51" s="23">
-        <v>0.3417</v>
-      </c>
-      <c r="I51" s="23">
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="J51" s="23">
-        <v>0.51039999999999996</v>
-      </c>
-      <c r="K51" s="23">
-        <v>0.59379999999999999</v>
-      </c>
-      <c r="L51" s="23">
-        <v>0.67730000000000001</v>
-      </c>
-      <c r="M51" s="23">
-        <v>0.76</v>
-      </c>
-      <c r="N51" s="23">
-        <v>0.7571</v>
-      </c>
-      <c r="O51" s="23">
-        <v>0.75560000000000005</v>
-      </c>
-      <c r="P51" s="23">
-        <v>0.75419999999999998</v>
-      </c>
-      <c r="Q51" s="23">
-        <v>0.75260000000000005</v>
-      </c>
-      <c r="R51" s="23">
-        <v>0.75009999999999999</v>
-      </c>
-      <c r="S51" s="23">
-        <v>0.74850000000000005</v>
-      </c>
-      <c r="T51" s="23">
-        <v>0.74709999999999999</v>
-      </c>
-      <c r="U51" s="23">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="V51" s="23">
-        <v>0.74439999999999995</v>
-      </c>
-      <c r="W51" s="23">
-        <v>0.74350000000000005</v>
-      </c>
-      <c r="X51" s="23">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="Y51" s="23">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="Z51" s="23">
-        <v>0.73929999999999996</v>
-      </c>
-      <c r="AA51" s="23">
-        <v>0.73809999999999998</v>
-      </c>
-      <c r="AB51" s="23">
-        <v>0.73570000000000002</v>
-      </c>
-      <c r="AC51" s="23">
-        <v>0.73440000000000005</v>
-      </c>
-      <c r="AD51" s="23">
-        <v>0.73409999999999997</v>
-      </c>
-      <c r="AE51" s="23">
-        <v>0.73260000000000003</v>
-      </c>
-      <c r="AF51" s="23">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="AG51" s="23">
-        <v>0.72960000000000003</v>
+      <c r="E51" s="20">
+        <v>0</v>
+      </c>
+      <c r="F51" s="20">
+        <v>0</v>
+      </c>
+      <c r="G51" s="20">
+        <v>0</v>
+      </c>
+      <c r="H51" s="20">
+        <v>0</v>
+      </c>
+      <c r="I51" s="20">
+        <v>0</v>
+      </c>
+      <c r="J51" s="20">
+        <v>0</v>
+      </c>
+      <c r="K51" s="20">
+        <v>0</v>
+      </c>
+      <c r="L51" s="20">
+        <v>0</v>
+      </c>
+      <c r="M51" s="20">
+        <v>0</v>
+      </c>
+      <c r="N51" s="20">
+        <v>0</v>
+      </c>
+      <c r="O51" s="20">
+        <v>0</v>
+      </c>
+      <c r="P51" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="20">
+        <v>0</v>
+      </c>
+      <c r="R51" s="20">
+        <v>0</v>
+      </c>
+      <c r="S51" s="20">
+        <v>0</v>
+      </c>
+      <c r="T51" s="20">
+        <v>0</v>
+      </c>
+      <c r="U51" s="20">
+        <v>0</v>
+      </c>
+      <c r="V51" s="20">
+        <v>0</v>
+      </c>
+      <c r="W51" s="20">
+        <v>0</v>
+      </c>
+      <c r="X51" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="20">
+        <v>0</v>
       </c>
       <c r="AH51" s="7"/>
       <c r="AI51" s="7"/>
@@ -39548,8 +39546,8 @@
   </sheetPr>
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="B2:AE8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39656,123 +39654,123 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="27">
         <v>0.05</v>
       </c>
-      <c r="C2" s="30">
-        <f>$B2</f>
+      <c r="C2" s="27">
+        <f t="shared" ref="C2:AE2" si="0">$B2</f>
         <v>0.05</v>
       </c>
-      <c r="D2" s="30">
-        <f>$B2</f>
+      <c r="D2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="E2" s="30">
-        <f>$B2</f>
+      <c r="E2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="F2" s="30">
-        <f>$B2</f>
+      <c r="F2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G2" s="30">
-        <f>$B2</f>
+      <c r="G2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="H2" s="30">
-        <f>$B2</f>
+      <c r="H2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="I2" s="30">
-        <f>$B2</f>
+      <c r="I2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="J2" s="30">
-        <f>$B2</f>
+      <c r="J2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="K2" s="30">
-        <f>$B2</f>
+      <c r="K2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="L2" s="30">
-        <f>$B2</f>
+      <c r="L2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M2" s="30">
-        <f>$B2</f>
+      <c r="M2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="N2" s="30">
-        <f>$B2</f>
+      <c r="N2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="O2" s="30">
-        <f>$B2</f>
+      <c r="O2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="P2" s="30">
-        <f>$B2</f>
+      <c r="P2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="Q2" s="30">
-        <f>$B2</f>
+      <c r="Q2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="R2" s="30">
-        <f>$B2</f>
+      <c r="R2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="S2" s="30">
-        <f>$B2</f>
+      <c r="S2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="T2" s="30">
-        <f>$B2</f>
+      <c r="T2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="U2" s="30">
-        <f>$B2</f>
+      <c r="U2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="V2" s="30">
-        <f>$B2</f>
+      <c r="V2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="W2" s="30">
-        <f>$B2</f>
+      <c r="W2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="X2" s="30">
-        <f>$B2</f>
+      <c r="X2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="Y2" s="30">
-        <f>$B2</f>
+      <c r="Y2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="Z2" s="30">
-        <f>$B2</f>
+      <c r="Z2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AA2" s="30">
-        <f>$B2</f>
+      <c r="AA2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AB2" s="30">
-        <f>$B2</f>
+      <c r="AB2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AC2" s="30">
-        <f>$B2</f>
+      <c r="AC2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AD2" s="30">
-        <f>$B2</f>
+      <c r="AD2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AE2" s="30">
-        <f>$B2</f>
+      <c r="AE2" s="27">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
     </row>
@@ -39780,219 +39778,219 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="27">
         <f>0.95-IRA!D51</f>
         <v>0.95</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="27">
         <f>0.95-IRA!E51</f>
-        <v>0.86309999999999998</v>
-      </c>
-      <c r="D3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="D3" s="27">
         <f>0.95-IRA!F51</f>
-        <v>0.77789999999999992</v>
-      </c>
-      <c r="E3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="E3" s="27">
         <f>0.95-IRA!G51</f>
-        <v>0.69279999999999997</v>
-      </c>
-      <c r="F3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="27">
         <f>0.95-IRA!H51</f>
-        <v>0.60829999999999995</v>
-      </c>
-      <c r="G3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="27">
         <f>0.95-IRA!I51</f>
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="H3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="H3" s="27">
         <f>0.95-IRA!J51</f>
-        <v>0.43959999999999999</v>
-      </c>
-      <c r="I3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="I3" s="27">
         <f>0.95-IRA!K51</f>
-        <v>0.35619999999999996</v>
-      </c>
-      <c r="J3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="J3" s="27">
         <f>0.95-IRA!L51</f>
-        <v>0.27269999999999994</v>
-      </c>
-      <c r="K3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="K3" s="27">
         <f>0.95-IRA!M51</f>
-        <v>0.18999999999999995</v>
-      </c>
-      <c r="L3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="L3" s="27">
         <f>0.95-IRA!N51</f>
-        <v>0.19289999999999996</v>
-      </c>
-      <c r="M3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="M3" s="27">
         <f>0.95-IRA!O51</f>
-        <v>0.19439999999999991</v>
-      </c>
-      <c r="N3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="N3" s="27">
         <f>0.95-IRA!P51</f>
-        <v>0.19579999999999997</v>
-      </c>
-      <c r="O3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="27">
         <f>0.95-IRA!Q51</f>
-        <v>0.19739999999999991</v>
-      </c>
-      <c r="P3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="P3" s="27">
         <f>0.95-IRA!R51</f>
-        <v>0.19989999999999997</v>
-      </c>
-      <c r="Q3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="Q3" s="27">
         <f>0.95-IRA!S51</f>
-        <v>0.2014999999999999</v>
-      </c>
-      <c r="R3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="R3" s="27">
         <f>0.95-IRA!T51</f>
-        <v>0.20289999999999997</v>
-      </c>
-      <c r="S3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="S3" s="27">
         <f>0.95-IRA!U51</f>
-        <v>0.2044999999999999</v>
-      </c>
-      <c r="T3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="T3" s="27">
         <f>0.95-IRA!V51</f>
-        <v>0.2056</v>
-      </c>
-      <c r="U3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="U3" s="27">
         <f>0.95-IRA!W51</f>
-        <v>0.20649999999999991</v>
-      </c>
-      <c r="V3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="V3" s="27">
         <f>0.95-IRA!X51</f>
-        <v>0.20699999999999996</v>
-      </c>
-      <c r="W3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="W3" s="27">
         <f>0.95-IRA!Y51</f>
-        <v>0.20799999999999996</v>
-      </c>
-      <c r="X3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="X3" s="27">
         <f>0.95-IRA!Z51</f>
-        <v>0.2107</v>
-      </c>
-      <c r="Y3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="Y3" s="27">
         <f>0.95-IRA!AA51</f>
-        <v>0.21189999999999998</v>
-      </c>
-      <c r="Z3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="Z3" s="27">
         <f>0.95-IRA!AB51</f>
-        <v>0.21429999999999993</v>
-      </c>
-      <c r="AA3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AA3" s="27">
         <f>0.95-IRA!AC51</f>
-        <v>0.2155999999999999</v>
-      </c>
-      <c r="AB3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AB3" s="27">
         <f>0.95-IRA!AD51</f>
-        <v>0.21589999999999998</v>
-      </c>
-      <c r="AC3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AC3" s="27">
         <f>0.95-IRA!AE51</f>
-        <v>0.21739999999999993</v>
-      </c>
-      <c r="AD3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AD3" s="27">
         <f>0.95-IRA!AF51</f>
-        <v>0.21899999999999997</v>
-      </c>
-      <c r="AE3" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AE3" s="27">
         <f>0.95-IRA!AG51</f>
-        <v>0.22039999999999993</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>0</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="27">
         <v>0</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="27">
         <v>0</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="27">
         <v>0</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="27">
         <v>0</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="27">
         <v>0</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="27">
         <v>0</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="27">
         <v>0</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="27">
         <v>0</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="27">
         <v>0</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="27">
         <v>0</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="27">
         <v>0</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="27">
         <v>0</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="27">
         <v>0</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="27">
         <v>0</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="Q4" s="27">
         <v>0</v>
       </c>
-      <c r="R4" s="30">
+      <c r="R4" s="27">
         <v>0</v>
       </c>
-      <c r="S4" s="30">
+      <c r="S4" s="27">
         <v>0</v>
       </c>
-      <c r="T4" s="30">
+      <c r="T4" s="27">
         <v>0</v>
       </c>
-      <c r="U4" s="30">
+      <c r="U4" s="27">
         <v>0</v>
       </c>
-      <c r="V4" s="30">
+      <c r="V4" s="27">
         <v>0</v>
       </c>
-      <c r="W4" s="30">
+      <c r="W4" s="27">
         <v>0</v>
       </c>
-      <c r="X4" s="30">
+      <c r="X4" s="27">
         <v>0</v>
       </c>
-      <c r="Y4" s="30">
+      <c r="Y4" s="27">
         <v>0</v>
       </c>
-      <c r="Z4" s="30">
+      <c r="Z4" s="27">
         <v>0</v>
       </c>
-      <c r="AA4" s="30">
+      <c r="AA4" s="27">
         <v>0</v>
       </c>
-      <c r="AB4" s="30">
+      <c r="AB4" s="27">
         <v>0</v>
       </c>
-      <c r="AC4" s="30">
+      <c r="AC4" s="27">
         <v>0</v>
       </c>
-      <c r="AD4" s="30">
+      <c r="AD4" s="27">
         <v>0</v>
       </c>
-      <c r="AE4" s="30">
+      <c r="AE4" s="27">
         <v>0</v>
       </c>
     </row>
@@ -40000,94 +39998,94 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="27">
         <v>0</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="27">
         <v>0</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="27">
         <v>0</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="27">
         <v>0</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="27">
         <v>0</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="27">
         <v>0</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="27">
         <v>0</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="27">
         <v>0</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="27">
         <v>0</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="27">
         <v>0</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="27">
         <v>0</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="27">
         <v>0</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="27">
         <v>0</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="27">
         <v>0</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="27">
         <v>0</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="27">
         <v>0</v>
       </c>
-      <c r="R5" s="30">
+      <c r="R5" s="27">
         <v>0</v>
       </c>
-      <c r="S5" s="30">
+      <c r="S5" s="27">
         <v>0</v>
       </c>
-      <c r="T5" s="30">
+      <c r="T5" s="27">
         <v>0</v>
       </c>
-      <c r="U5" s="30">
+      <c r="U5" s="27">
         <v>0</v>
       </c>
-      <c r="V5" s="30">
+      <c r="V5" s="27">
         <v>0</v>
       </c>
-      <c r="W5" s="30">
+      <c r="W5" s="27">
         <v>0</v>
       </c>
-      <c r="X5" s="30">
+      <c r="X5" s="27">
         <v>0</v>
       </c>
-      <c r="Y5" s="30">
+      <c r="Y5" s="27">
         <v>0</v>
       </c>
-      <c r="Z5" s="30">
+      <c r="Z5" s="27">
         <v>0</v>
       </c>
-      <c r="AA5" s="30">
+      <c r="AA5" s="27">
         <v>0</v>
       </c>
-      <c r="AB5" s="30">
+      <c r="AB5" s="27">
         <v>0</v>
       </c>
-      <c r="AC5" s="30">
+      <c r="AC5" s="27">
         <v>0</v>
       </c>
-      <c r="AD5" s="30">
+      <c r="AD5" s="27">
         <v>0</v>
       </c>
-      <c r="AE5" s="30">
+      <c r="AE5" s="27">
         <v>0</v>
       </c>
     </row>
@@ -40095,94 +40093,94 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="27">
         <v>0</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="27">
         <v>0</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="27">
         <v>0</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="27">
         <v>0</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="27">
         <v>0</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="27">
         <v>0</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="27">
         <v>0</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="27">
         <v>0</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="27">
         <v>0</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="27">
         <v>0</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="27">
         <v>0</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="27">
         <v>0</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="27">
         <v>0</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="27">
         <v>0</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="27">
         <v>0</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="27">
         <v>0</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="27">
         <v>0</v>
       </c>
-      <c r="S6" s="30">
+      <c r="S6" s="27">
         <v>0</v>
       </c>
-      <c r="T6" s="30">
+      <c r="T6" s="27">
         <v>0</v>
       </c>
-      <c r="U6" s="30">
+      <c r="U6" s="27">
         <v>0</v>
       </c>
-      <c r="V6" s="30">
+      <c r="V6" s="27">
         <v>0</v>
       </c>
-      <c r="W6" s="30">
+      <c r="W6" s="27">
         <v>0</v>
       </c>
-      <c r="X6" s="30">
+      <c r="X6" s="27">
         <v>0</v>
       </c>
-      <c r="Y6" s="30">
+      <c r="Y6" s="27">
         <v>0</v>
       </c>
-      <c r="Z6" s="30">
+      <c r="Z6" s="27">
         <v>0</v>
       </c>
-      <c r="AA6" s="30">
+      <c r="AA6" s="27">
         <v>0</v>
       </c>
-      <c r="AB6" s="30">
+      <c r="AB6" s="27">
         <v>0</v>
       </c>
-      <c r="AC6" s="30">
+      <c r="AC6" s="27">
         <v>0</v>
       </c>
-      <c r="AD6" s="30">
+      <c r="AD6" s="27">
         <v>0</v>
       </c>
-      <c r="AE6" s="30">
+      <c r="AE6" s="27">
         <v>0</v>
       </c>
     </row>
@@ -40190,219 +40188,219 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="27">
         <f>IRA!D51</f>
         <v>0</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="27">
         <f>IRA!E51</f>
-        <v>8.6900000000000005E-2</v>
-      </c>
-      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="D7" s="27">
         <f>IRA!F51</f>
-        <v>0.1721</v>
-      </c>
-      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="27">
         <f>IRA!G51</f>
-        <v>0.25719999999999998</v>
-      </c>
-      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
         <f>IRA!H51</f>
-        <v>0.3417</v>
-      </c>
-      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
         <f>IRA!I51</f>
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="27">
         <f>IRA!J51</f>
-        <v>0.51039999999999996</v>
-      </c>
-      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27">
         <f>IRA!K51</f>
-        <v>0.59379999999999999</v>
-      </c>
-      <c r="J7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="27">
         <f>IRA!L51</f>
-        <v>0.67730000000000001</v>
-      </c>
-      <c r="K7" s="30">
+        <v>0</v>
+      </c>
+      <c r="K7" s="27">
         <f>IRA!M51</f>
-        <v>0.76</v>
-      </c>
-      <c r="L7" s="30">
+        <v>0</v>
+      </c>
+      <c r="L7" s="27">
         <f>IRA!N51</f>
-        <v>0.7571</v>
-      </c>
-      <c r="M7" s="30">
+        <v>0</v>
+      </c>
+      <c r="M7" s="27">
         <f>IRA!O51</f>
-        <v>0.75560000000000005</v>
-      </c>
-      <c r="N7" s="30">
+        <v>0</v>
+      </c>
+      <c r="N7" s="27">
         <f>IRA!P51</f>
-        <v>0.75419999999999998</v>
-      </c>
-      <c r="O7" s="30">
+        <v>0</v>
+      </c>
+      <c r="O7" s="27">
         <f>IRA!Q51</f>
-        <v>0.75260000000000005</v>
-      </c>
-      <c r="P7" s="30">
+        <v>0</v>
+      </c>
+      <c r="P7" s="27">
         <f>IRA!R51</f>
-        <v>0.75009999999999999</v>
-      </c>
-      <c r="Q7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="27">
         <f>IRA!S51</f>
-        <v>0.74850000000000005</v>
-      </c>
-      <c r="R7" s="30">
+        <v>0</v>
+      </c>
+      <c r="R7" s="27">
         <f>IRA!T51</f>
-        <v>0.74709999999999999</v>
-      </c>
-      <c r="S7" s="30">
+        <v>0</v>
+      </c>
+      <c r="S7" s="27">
         <f>IRA!U51</f>
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="T7" s="30">
+        <v>0</v>
+      </c>
+      <c r="T7" s="27">
         <f>IRA!V51</f>
-        <v>0.74439999999999995</v>
-      </c>
-      <c r="U7" s="30">
+        <v>0</v>
+      </c>
+      <c r="U7" s="27">
         <f>IRA!W51</f>
-        <v>0.74350000000000005</v>
-      </c>
-      <c r="V7" s="30">
+        <v>0</v>
+      </c>
+      <c r="V7" s="27">
         <f>IRA!X51</f>
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="W7" s="30">
+        <v>0</v>
+      </c>
+      <c r="W7" s="27">
         <f>IRA!Y51</f>
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="X7" s="30">
+        <v>0</v>
+      </c>
+      <c r="X7" s="27">
         <f>IRA!Z51</f>
-        <v>0.73929999999999996</v>
-      </c>
-      <c r="Y7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="27">
         <f>IRA!AA51</f>
-        <v>0.73809999999999998</v>
-      </c>
-      <c r="Z7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="27">
         <f>IRA!AB51</f>
-        <v>0.73570000000000002</v>
-      </c>
-      <c r="AA7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="27">
         <f>IRA!AC51</f>
-        <v>0.73440000000000005</v>
-      </c>
-      <c r="AB7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="27">
         <f>IRA!AD51</f>
-        <v>0.73409999999999997</v>
-      </c>
-      <c r="AC7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="27">
         <f>IRA!AE51</f>
-        <v>0.73260000000000003</v>
-      </c>
-      <c r="AD7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="27">
         <f>IRA!AF51</f>
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="AE7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="27">
         <f>IRA!AG51</f>
-        <v>0.72960000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="27">
         <v>0</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="27">
         <v>0</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="27">
         <v>0</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="27">
         <v>0</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="27">
         <v>0</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="27">
         <v>0</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="27">
         <v>0</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="27">
         <v>0</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="27">
         <v>0</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="27">
         <v>0</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="27">
         <v>0</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="27">
         <v>0</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="27">
         <v>0</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="27">
         <v>0</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="27">
         <v>0</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="27">
         <v>0</v>
       </c>
-      <c r="R8" s="30">
+      <c r="R8" s="27">
         <v>0</v>
       </c>
-      <c r="S8" s="30">
+      <c r="S8" s="27">
         <v>0</v>
       </c>
-      <c r="T8" s="30">
+      <c r="T8" s="27">
         <v>0</v>
       </c>
-      <c r="U8" s="30">
+      <c r="U8" s="27">
         <v>0</v>
       </c>
-      <c r="V8" s="30">
+      <c r="V8" s="27">
         <v>0</v>
       </c>
-      <c r="W8" s="30">
+      <c r="W8" s="27">
         <v>0</v>
       </c>
-      <c r="X8" s="30">
+      <c r="X8" s="27">
         <v>0</v>
       </c>
-      <c r="Y8" s="30">
+      <c r="Y8" s="27">
         <v>0</v>
       </c>
-      <c r="Z8" s="30">
+      <c r="Z8" s="27">
         <v>0</v>
       </c>
-      <c r="AA8" s="30">
+      <c r="AA8" s="27">
         <v>0</v>
       </c>
-      <c r="AB8" s="30">
+      <c r="AB8" s="27">
         <v>0</v>
       </c>
-      <c r="AC8" s="30">
+      <c r="AC8" s="27">
         <v>0</v>
       </c>
-      <c r="AD8" s="30">
+      <c r="AD8" s="27">
         <v>0</v>
       </c>
-      <c r="AE8" s="30">
+      <c r="AE8" s="27">
         <v>0</v>
       </c>
     </row>

</xml_diff>